<commit_message>
login & reset password
</commit_message>
<xml_diff>
--- a/excel/Data Simpanan.xlsx
+++ b/excel/Data Simpanan.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>No Kartu</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Tumbang miwan</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>T.II/WH/0002</t>
   </si>
 </sst>
 </file>
@@ -423,7 +429,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,10 +518,10 @@
         <v>5000</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -545,7 +551,63 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>55000</v>
+        <v>65000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>50000</v>
+      </c>
+      <c r="F4">
+        <v>5000</v>
+      </c>
+      <c r="G4">
+        <v>5000</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>60000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>